<commit_message>
Added error handling on file upload and validation code
</commit_message>
<xml_diff>
--- a/www/Packaging Models Dataset Sample.xlsx
+++ b/www/Packaging Models Dataset Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Model Builder\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE73534B-A86C-4422-AA4F-2F8BAFEFEE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABCE43-DF81-4E5A-A8EE-A9DAAD1EA3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="16185" windowHeight="12180" activeTab="1" xr2:uid="{19036D93-B832-48DA-965B-463EFCD7E34A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19036D93-B832-48DA-965B-463EFCD7E34A}"/>
   </bookViews>
   <sheets>
     <sheet name="stack_3" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="42">
   <si>
     <t>Stack</t>
   </si>
@@ -182,12 +182,15 @@
   <si>
     <t>Layer_1_thickness_gsm</t>
   </si>
+  <si>
+    <t>Validation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,12 +215,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
     </font>
   </fonts>
   <fills count="3">
@@ -247,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -258,7 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54C8C29-6AC8-4749-9AB6-0F897BD402E5}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -671,7 +667,9 @@
       <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="10"/>
+      <c r="S1" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
@@ -728,6 +726,9 @@
       <c r="R2">
         <v>7.1079397201538086</v>
       </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
@@ -784,6 +785,9 @@
       <c r="R3">
         <v>2.2224209308624268</v>
       </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
@@ -840,6 +844,9 @@
       <c r="R4">
         <v>3.8996126651763916</v>
       </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
@@ -896,6 +903,9 @@
       <c r="R5">
         <v>8.6601543426513672</v>
       </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
@@ -952,6 +962,9 @@
       <c r="R6">
         <v>7.98992919921875</v>
       </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
@@ -1008,6 +1021,9 @@
       <c r="R7">
         <v>11.026665687561035</v>
       </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
@@ -1064,6 +1080,9 @@
       <c r="R8">
         <v>10.77735710144043</v>
       </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
@@ -1120,6 +1139,9 @@
       <c r="R9">
         <v>9.1216840744018555</v>
       </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
@@ -1176,6 +1198,9 @@
       <c r="R10">
         <v>8.8586311340332031</v>
       </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
@@ -1232,6 +1257,9 @@
       <c r="R11">
         <v>9.5267162322998047</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
@@ -1288,6 +1316,9 @@
       <c r="R12">
         <v>11.152593612670898</v>
       </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
@@ -1344,6 +1375,9 @@
       <c r="R13">
         <v>8.9457120895385742</v>
       </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
@@ -1400,6 +1434,9 @@
       <c r="R14">
         <v>9.6833610534667969</v>
       </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
@@ -1456,6 +1493,9 @@
       <c r="R15">
         <v>9.0160083770751953</v>
       </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
@@ -1511,6 +1551,9 @@
       </c>
       <c r="R16">
         <v>11.638176918029785</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1523,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA0BC33-B8F0-4CD2-82D6-B2E77C717B18}">
-  <dimension ref="A1:W757"/>
+  <dimension ref="A1:X757"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1554,7 +1597,7 @@
     <col min="22" max="22" width="12.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1624,8 +1667,11 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1690,8 +1736,11 @@
       <c r="W2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1732,7 +1781,7 @@
         <v>120</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N66" si="0">O3/4</f>
+        <f t="shared" ref="N3:N13" si="0">O3/4</f>
         <v>38.5</v>
       </c>
       <c r="O3">
@@ -1753,8 +1802,11 @@
       <c r="V3" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1816,8 +1868,11 @@
       <c r="V4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="X4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1867,8 +1922,11 @@
       <c r="P5">
         <v>500</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1918,8 +1976,11 @@
       <c r="P6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="X6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1969,8 +2030,11 @@
       <c r="P7">
         <v>500</v>
       </c>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2034,8 +2098,11 @@
       <c r="V8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2097,8 +2164,11 @@
       <c r="V9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2162,8 +2232,11 @@
       <c r="V10" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="X10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2217,7 +2290,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2268,7 +2341,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2319,7 +2392,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:24">
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -2327,7 +2400,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:24">
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -2335,7 +2408,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:24">
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -5048,6 +5121,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002492EA91F8B12B4EBF4F32A47DC26525" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d326a81ef988979cf445b7c467541a4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2dac8b6-24e8-4e87-b4bb-f7ce6e9e0cbb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbed2a2dcc2cdcba095f135437a72f54" ns2:_="">
     <xsd:import namespace="e2dac8b6-24e8-4e87-b4bb-f7ce6e9e0cbb"/>
@@ -5231,15 +5313,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F70483F0-C98B-403E-9932-AE7E5968E173}">
   <ds:schemaRefs>
@@ -5250,6 +5323,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E826A088-D8D2-4841-8616-E34F04D08FA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51B7912-847B-41FD-AACC-EF417A17292B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5265,12 +5346,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E826A088-D8D2-4841-8616-E34F04D08FA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>